<commit_message>
MAJ moteur avant + avancement dans les règles
Mise à jour du moteur avant (prise en compte d'un attribut dans les
faits déjà existant)
</commit_message>
<xml_diff>
--- a/[RECUEIL] Général.xlsx
+++ b/[RECUEIL] Général.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="20490" windowHeight="7890"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="20490" windowHeight="7890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MAMMIFERES" sheetId="2" r:id="rId1"/>
@@ -1921,7 +1921,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1965,72 +1965,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2046,66 +1980,12 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2121,37 +2001,10 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2160,25 +2013,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2190,42 +2025,18 @@
     <xf numFmtId="0" fontId="25" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2235,30 +2046,12 @@
     <xf numFmtId="0" fontId="24" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2267,6 +2060,219 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2592,8 +2598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.85546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2608,785 +2614,785 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="70" t="s">
+      <c r="F1" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="67" t="s">
+      <c r="G1" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="68" t="s">
+      <c r="A2" s="54"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="73" t="s">
+      <c r="E2" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="70" t="s">
+      <c r="F2" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="72"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="72"/>
-      <c r="B3" s="72"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="75" t="s">
+      <c r="A3" s="54"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="76" t="s">
+      <c r="E3" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="77" t="s">
+      <c r="F3" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="74"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="72"/>
-      <c r="B4" s="72"/>
-      <c r="C4" s="67" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="69" t="s">
+      <c r="E4" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="70" t="s">
+      <c r="F4" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="67" t="s">
+      <c r="G4" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="72"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="75" t="s">
+      <c r="A5" s="54"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="78" t="s">
+      <c r="E5" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="77" t="s">
+      <c r="F5" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="72"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="72"/>
-      <c r="B6" s="67" t="s">
+      <c r="A6" s="54"/>
+      <c r="B6" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="67" t="s">
+      <c r="C6" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="75" t="s">
+      <c r="D6" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="79" t="s">
+      <c r="E6" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="80" t="s">
+      <c r="F6" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="72"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="72"/>
-      <c r="B7" s="72"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="75" t="s">
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="79" t="s">
+      <c r="E7" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="81"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="62" t="s">
+      <c r="F7" s="50"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="22" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="72"/>
-      <c r="B8" s="72"/>
-      <c r="C8" s="67" t="s">
+      <c r="A8" s="54"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="75" t="s">
+      <c r="D8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="78" t="s">
+      <c r="E8" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="82" t="s">
+      <c r="F8" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="72"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="63" t="s">
+      <c r="G8" s="54"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="23" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="72"/>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="75" t="s">
+      <c r="A9" s="54"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="78" t="s">
+      <c r="E9" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="83"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="64" t="s">
+      <c r="F9" s="51"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="24" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="72"/>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="75" t="s">
+      <c r="A10" s="54"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="79" t="s">
+      <c r="E10" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="80" t="s">
+      <c r="F10" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="72"/>
-      <c r="H10" s="71"/>
-      <c r="I10" s="71"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="72"/>
-      <c r="B11" s="72"/>
-      <c r="C11" s="72"/>
-      <c r="D11" s="75" t="s">
+      <c r="A11" s="54"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="79" t="s">
+      <c r="E11" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="81"/>
-      <c r="G11" s="72"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="72"/>
-      <c r="B12" s="72"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="75" t="s">
+      <c r="A12" s="54"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="79" t="s">
+      <c r="E12" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="83"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="71"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="72"/>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="75" t="s">
+      <c r="A13" s="54"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="79" t="s">
+      <c r="E13" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="80" t="s">
+      <c r="F13" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="72"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="71"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="72"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="75" t="s">
+      <c r="A14" s="54"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="79" t="s">
+      <c r="E14" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="81"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="71"/>
-      <c r="I14" s="71"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="72"/>
-      <c r="B15" s="74"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="75" t="s">
+      <c r="A15" s="54"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="79" t="s">
+      <c r="E15" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="83"/>
-      <c r="G15" s="72"/>
-      <c r="H15" s="71"/>
-      <c r="I15" s="71"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="72"/>
-      <c r="B16" s="67" t="s">
+      <c r="A16" s="54"/>
+      <c r="B16" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="75" t="s">
+      <c r="D16" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="79" t="s">
+      <c r="E16" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="80" t="s">
+      <c r="F16" s="111" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="72"/>
-      <c r="H16" s="71"/>
-      <c r="I16" s="71"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="74"/>
-      <c r="B17" s="74"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="75" t="s">
+      <c r="A17" s="55"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="110"/>
+      <c r="D17" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="84" t="s">
+      <c r="E17" s="113" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="83"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="71"/>
-      <c r="I17" s="71"/>
+      <c r="F17" s="112"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="98" t="s">
+      <c r="A18" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="98" t="s">
+      <c r="B18" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="104" t="s">
+      <c r="C18" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="105"/>
-      <c r="E18" s="113" t="s">
+      <c r="D18" s="47"/>
+      <c r="E18" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="F18" s="94" t="s">
+      <c r="F18" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="G18" s="98" t="s">
+      <c r="G18" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="67" t="s">
+      <c r="H18" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="I18" s="71"/>
+      <c r="I18" s="27"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="99"/>
-      <c r="B19" s="99"/>
-      <c r="C19" s="106"/>
-      <c r="D19" s="107"/>
-      <c r="E19" s="101" t="s">
+      <c r="A19" s="57"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="103" t="s">
+      <c r="F19" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="99"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="71"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="27"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="99"/>
-      <c r="B20" s="99"/>
-      <c r="C20" s="108"/>
-      <c r="D20" s="109"/>
-      <c r="E20" s="101" t="s">
+      <c r="A20" s="57"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="103" t="s">
+      <c r="F20" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="G20" s="100"/>
-      <c r="H20" s="72"/>
-      <c r="I20" s="71"/>
+      <c r="G20" s="66"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="27"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="99"/>
-      <c r="B21" s="99"/>
-      <c r="C21" s="98" t="s">
+      <c r="A21" s="57"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="98" t="s">
+      <c r="D21" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="E21" s="101" t="s">
+      <c r="E21" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="103" t="s">
+      <c r="F21" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="G21" s="105" t="s">
+      <c r="G21" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="H21" s="72"/>
-      <c r="I21" s="71"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="27"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="99"/>
-      <c r="B22" s="100"/>
-      <c r="C22" s="100"/>
-      <c r="D22" s="100"/>
-      <c r="E22" s="114" t="s">
+      <c r="A22" s="57"/>
+      <c r="B22" s="66"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="F22" s="115" t="s">
+      <c r="F22" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="G22" s="109"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="71"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="27"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="99"/>
-      <c r="B23" s="98" t="s">
+      <c r="A23" s="57"/>
+      <c r="B23" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="98" t="s">
+      <c r="C23" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="98" t="s">
+      <c r="D23" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="E23" s="101" t="s">
+      <c r="E23" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="F23" s="103" t="s">
+      <c r="F23" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="G23" s="101" t="s">
+      <c r="G23" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="H23" s="72"/>
-      <c r="I23" s="71"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="27"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="99"/>
-      <c r="B24" s="99"/>
-      <c r="C24" s="99"/>
-      <c r="D24" s="100"/>
-      <c r="E24" s="111" t="s">
+      <c r="A24" s="57"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="43" t="s">
         <v>228</v>
       </c>
-      <c r="F24" s="103" t="s">
+      <c r="F24" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="G24" s="98" t="s">
+      <c r="G24" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="H24" s="72"/>
-      <c r="I24" s="71"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="27"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="99"/>
-      <c r="B25" s="99"/>
-      <c r="C25" s="99"/>
-      <c r="D25" s="101" t="s">
+      <c r="A25" s="57"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="E25" s="101" t="s">
+      <c r="E25" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="103" t="s">
+      <c r="F25" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="G25" s="99"/>
-      <c r="H25" s="72"/>
-      <c r="I25" s="71"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="27"/>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="99"/>
-      <c r="B26" s="99"/>
-      <c r="C26" s="99"/>
-      <c r="D26" s="98" t="s">
+      <c r="A26" s="57"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="101" t="s">
+      <c r="E26" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="F26" s="103" t="s">
+      <c r="F26" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="G26" s="99"/>
-      <c r="H26" s="72"/>
-      <c r="I26" s="71"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="27"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="99"/>
-      <c r="B27" s="99"/>
-      <c r="C27" s="99"/>
-      <c r="D27" s="99"/>
-      <c r="E27" s="101" t="s">
+      <c r="A27" s="57"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="F27" s="103" t="s">
+      <c r="F27" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="G27" s="99"/>
-      <c r="H27" s="72"/>
-      <c r="I27" s="71"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="27"/>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="99"/>
-      <c r="B28" s="99"/>
-      <c r="C28" s="99"/>
-      <c r="D28" s="99"/>
-      <c r="E28" s="111" t="s">
+      <c r="A28" s="57"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="43" t="s">
         <v>231</v>
       </c>
-      <c r="F28" s="103" t="s">
+      <c r="F28" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="G28" s="99"/>
-      <c r="H28" s="72"/>
-      <c r="I28" s="71"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="27"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="99"/>
-      <c r="B29" s="99"/>
-      <c r="C29" s="99"/>
-      <c r="D29" s="99"/>
-      <c r="E29" s="111" t="s">
+      <c r="A29" s="57"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="43" t="s">
         <v>230</v>
       </c>
-      <c r="F29" s="103" t="s">
+      <c r="F29" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="G29" s="99"/>
-      <c r="H29" s="72"/>
-      <c r="I29" s="71"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="27"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="99"/>
-      <c r="B30" s="99"/>
-      <c r="C30" s="99"/>
-      <c r="D30" s="99"/>
-      <c r="E30" s="87" t="s">
+      <c r="A30" s="57"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="32" t="s">
         <v>229</v>
       </c>
-      <c r="F30" s="88" t="s">
+      <c r="F30" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="G30" s="99"/>
-      <c r="H30" s="72"/>
-      <c r="I30" s="71"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="54"/>
+      <c r="I30" s="27"/>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="99"/>
-      <c r="B31" s="99"/>
-      <c r="C31" s="100"/>
-      <c r="D31" s="100"/>
-      <c r="E31" s="101" t="s">
+      <c r="A31" s="57"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="103" t="s">
+      <c r="F31" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="G31" s="100"/>
-      <c r="H31" s="72"/>
-      <c r="I31" s="71"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="54"/>
+      <c r="I31" s="27"/>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="100"/>
-      <c r="B32" s="100"/>
-      <c r="C32" s="101" t="s">
+      <c r="A32" s="66"/>
+      <c r="B32" s="66"/>
+      <c r="C32" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="101" t="s">
+      <c r="D32" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="E32" s="101" t="s">
+      <c r="E32" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="F32" s="103" t="s">
+      <c r="F32" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="G32" s="101" t="s">
+      <c r="G32" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H32" s="74"/>
-      <c r="I32" s="71"/>
+      <c r="H32" s="55"/>
+      <c r="I32" s="27"/>
     </row>
     <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="98" t="s">
+      <c r="A33" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="B33" s="90" t="s">
+      <c r="B33" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="104" t="s">
+      <c r="C33" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D33" s="105"/>
-      <c r="E33" s="101" t="s">
+      <c r="D33" s="47"/>
+      <c r="E33" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="F33" s="103" t="s">
+      <c r="F33" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="G33" s="104" t="s">
+      <c r="G33" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="H33" s="105"/>
-      <c r="I33" s="75" t="s">
+      <c r="H33" s="47"/>
+      <c r="I33" s="28" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="99"/>
-      <c r="B34" s="91"/>
-      <c r="C34" s="108"/>
-      <c r="D34" s="109"/>
-      <c r="E34" s="87" t="s">
+      <c r="A34" s="57"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="F34" s="88" t="s">
+      <c r="F34" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="G34" s="108"/>
-      <c r="H34" s="109"/>
-      <c r="I34" s="85"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="31"/>
     </row>
     <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="99"/>
-      <c r="B35" s="91"/>
-      <c r="C35" s="104" t="s">
+      <c r="A35" s="57"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="105"/>
-      <c r="E35" s="101" t="s">
+      <c r="D35" s="47"/>
+      <c r="E35" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="F35" s="103" t="s">
+      <c r="F35" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="G35" s="98" t="s">
+      <c r="G35" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="H35" s="98" t="s">
+      <c r="H35" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="I35" s="67" t="s">
+      <c r="I35" s="53" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="99"/>
-      <c r="B36" s="91"/>
-      <c r="C36" s="106"/>
-      <c r="D36" s="107"/>
-      <c r="E36" s="101" t="s">
+      <c r="A36" s="57"/>
+      <c r="B36" s="60"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="F36" s="110" t="s">
+      <c r="F36" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="G36" s="99"/>
-      <c r="H36" s="99"/>
-      <c r="I36" s="72"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="54"/>
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="99"/>
-      <c r="B37" s="91"/>
-      <c r="C37" s="108"/>
-      <c r="D37" s="109"/>
-      <c r="E37" s="101" t="s">
+      <c r="A37" s="57"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="F37" s="103" t="s">
+      <c r="F37" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="G37" s="100"/>
-      <c r="H37" s="99"/>
-      <c r="I37" s="72"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="54"/>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="99"/>
-      <c r="B38" s="91"/>
-      <c r="C38" s="98" t="s">
+      <c r="A38" s="57"/>
+      <c r="B38" s="60"/>
+      <c r="C38" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="D38" s="98" t="s">
+      <c r="D38" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="E38" s="101" t="s">
+      <c r="E38" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="F38" s="103" t="s">
+      <c r="F38" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="G38" s="98" t="s">
+      <c r="G38" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="H38" s="99"/>
-      <c r="I38" s="72"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="54"/>
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="99"/>
-      <c r="B39" s="91"/>
-      <c r="C39" s="99"/>
-      <c r="D39" s="99"/>
-      <c r="E39" s="87" t="s">
+      <c r="A39" s="57"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="F39" s="88" t="s">
+      <c r="F39" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="G39" s="99"/>
-      <c r="H39" s="99"/>
-      <c r="I39" s="72"/>
+      <c r="G39" s="57"/>
+      <c r="H39" s="57"/>
+      <c r="I39" s="54"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="99"/>
-      <c r="B40" s="91"/>
-      <c r="C40" s="99"/>
-      <c r="D40" s="100"/>
-      <c r="E40" s="101" t="s">
+      <c r="A40" s="57"/>
+      <c r="B40" s="60"/>
+      <c r="C40" s="57"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="F40" s="103" t="s">
+      <c r="F40" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="G40" s="99"/>
-      <c r="H40" s="99"/>
-      <c r="I40" s="72"/>
+      <c r="G40" s="57"/>
+      <c r="H40" s="57"/>
+      <c r="I40" s="54"/>
     </row>
     <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="99"/>
-      <c r="B41" s="91"/>
-      <c r="C41" s="99"/>
-      <c r="D41" s="98" t="s">
+      <c r="A41" s="57"/>
+      <c r="B41" s="60"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="E41" s="101" t="s">
+      <c r="E41" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="F41" s="102" t="s">
+      <c r="F41" s="39" t="s">
         <v>226</v>
       </c>
-      <c r="G41" s="99"/>
-      <c r="H41" s="99"/>
-      <c r="I41" s="72"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="54"/>
     </row>
     <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="99"/>
-      <c r="B42" s="91"/>
-      <c r="C42" s="99"/>
-      <c r="D42" s="100"/>
-      <c r="E42" s="101" t="s">
+      <c r="A42" s="57"/>
+      <c r="B42" s="60"/>
+      <c r="C42" s="57"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="F42" s="103" t="s">
+      <c r="F42" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="G42" s="99"/>
-      <c r="H42" s="99"/>
-      <c r="I42" s="72"/>
+      <c r="G42" s="57"/>
+      <c r="H42" s="57"/>
+      <c r="I42" s="54"/>
     </row>
     <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="99"/>
-      <c r="B43" s="92"/>
-      <c r="C43" s="100"/>
-      <c r="D43" s="101" t="s">
+      <c r="A43" s="57"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="E43" s="101" t="s">
+      <c r="E43" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="F43" s="103" t="s">
+      <c r="F43" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="G43" s="100"/>
-      <c r="H43" s="100"/>
-      <c r="I43" s="72"/>
+      <c r="G43" s="66"/>
+      <c r="H43" s="66"/>
+      <c r="I43" s="54"/>
     </row>
     <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="112"/>
-      <c r="B44" s="89" t="s">
+      <c r="A44" s="58"/>
+      <c r="B44" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="C44" s="95" t="s">
+      <c r="C44" s="68" t="s">
         <v>119</v>
       </c>
-      <c r="D44" s="96"/>
-      <c r="E44" s="93" t="s">
+      <c r="D44" s="69"/>
+      <c r="E44" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="F44" s="97" t="s">
+      <c r="F44" s="37" t="s">
         <v>225</v>
       </c>
-      <c r="G44" s="95" t="s">
+      <c r="G44" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="H44" s="96"/>
-      <c r="I44" s="86"/>
+      <c r="H44" s="69"/>
+      <c r="I44" s="67"/>
     </row>
     <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
@@ -3566,17 +3572,18 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G4:G17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A33:A44"/>
-    <mergeCell ref="B33:B43"/>
-    <mergeCell ref="C33:D34"/>
-    <mergeCell ref="C35:D37"/>
-    <mergeCell ref="C38:C43"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="D26:D31"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="G24:G31"/>
+    <mergeCell ref="B23:B32"/>
+    <mergeCell ref="C23:C31"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="C18:D20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C8:C15"/>
     <mergeCell ref="B6:B15"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="C21:C22"/>
@@ -3593,22 +3600,21 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="H18:H32"/>
     <mergeCell ref="F16:F17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A33:A44"/>
+    <mergeCell ref="B33:B43"/>
+    <mergeCell ref="C33:D34"/>
+    <mergeCell ref="C35:D37"/>
+    <mergeCell ref="C38:C43"/>
     <mergeCell ref="A1:A17"/>
     <mergeCell ref="B1:B5"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="A18:A32"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="D26:D31"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="G24:G31"/>
-    <mergeCell ref="B23:B32"/>
-    <mergeCell ref="C23:C31"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="C18:D20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C8:C15"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G4:G17"/>
   </mergeCells>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3619,7 +3625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -3630,303 +3636,303 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="91" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="93" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="40" t="s">
+      <c r="C1" s="106"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="20" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="61"/>
-      <c r="B2" s="52" t="s">
+      <c r="A2" s="105"/>
+      <c r="B2" s="91" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="91" t="s">
         <v>125</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="91" t="s">
         <v>126</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="F2" s="21" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="61"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="37" t="s">
+      <c r="A3" s="105"/>
+      <c r="B3" s="105"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="16" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="61"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="40" t="s">
+      <c r="A4" s="105"/>
+      <c r="B4" s="105"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="F4" s="65" t="s">
+      <c r="F4" s="25" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="61"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="40" t="s">
+      <c r="A5" s="105"/>
+      <c r="B5" s="105"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="F5" s="66" t="s">
+      <c r="F5" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="H5" s="62" t="s">
+      <c r="H5" s="22" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="61"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="40" t="s">
+      <c r="A6" s="105"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="F6" s="53" t="s">
+      <c r="F6" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="H6" s="63" t="s">
+      <c r="H6" s="23" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="61"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="40" t="s">
+      <c r="A7" s="105"/>
+      <c r="B7" s="105"/>
+      <c r="C7" s="105"/>
+      <c r="D7" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="53" t="s">
+      <c r="F7" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="H7" s="64" t="s">
+      <c r="H7" s="24" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="61"/>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="57" t="s">
+      <c r="A8" s="105"/>
+      <c r="B8" s="105"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="107" t="s">
         <v>224</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="F8" s="53" t="s">
+      <c r="F8" s="21" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="61"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="40" t="s">
+      <c r="A9" s="105"/>
+      <c r="B9" s="105"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="108"/>
+      <c r="E9" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="53" t="s">
+      <c r="F9" s="21" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="61"/>
-      <c r="B10" s="61"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="40" t="s">
+      <c r="A10" s="105"/>
+      <c r="B10" s="105"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="108"/>
+      <c r="E10" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="F10" s="53" t="s">
+      <c r="F10" s="21" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="61"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="40" t="s">
+      <c r="A11" s="105"/>
+      <c r="B11" s="105"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="109"/>
+      <c r="E11" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="F11" s="53" t="s">
+      <c r="F11" s="21" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="61"/>
-      <c r="B12" s="61"/>
-      <c r="C12" s="52" t="s">
+      <c r="A12" s="105"/>
+      <c r="B12" s="105"/>
+      <c r="C12" s="91" t="s">
         <v>141</v>
       </c>
-      <c r="D12" s="52" t="s">
+      <c r="D12" s="91" t="s">
         <v>142</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="53" t="s">
+      <c r="F12" s="21" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="61"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="40" t="s">
+      <c r="A13" s="105"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="92"/>
+      <c r="E13" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="F13" s="53" t="s">
+      <c r="F13" s="21" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="40" t="s">
+      <c r="A14" s="92"/>
+      <c r="B14" s="92"/>
+      <c r="C14" s="92"/>
+      <c r="D14" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="39" t="s">
+      <c r="F14" s="17" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="82" t="s">
         <v>146</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="40" t="s">
+      <c r="B15" s="83"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="F15" s="41" t="s">
+      <c r="F15" s="19" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="40" t="s">
+      <c r="A16" s="85"/>
+      <c r="B16" s="86"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="F16" s="41" t="s">
+      <c r="F16" s="19" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="40" t="s">
+      <c r="A17" s="85"/>
+      <c r="B17" s="86"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="41" t="s">
+      <c r="F17" s="19" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="48"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="37" t="s">
+      <c r="A18" s="88"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="90"/>
+      <c r="E18" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="38" t="s">
+      <c r="F18" s="16" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="82" t="s">
         <v>152</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="42" t="s">
+      <c r="B19" s="84"/>
+      <c r="C19" s="82" t="s">
         <v>153</v>
       </c>
-      <c r="D19" s="44"/>
-      <c r="E19" s="52" t="s">
+      <c r="D19" s="84"/>
+      <c r="E19" s="91" t="s">
         <v>154</v>
       </c>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="21" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="45"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="38" t="s">
+      <c r="A20" s="85"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="88"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="92"/>
+      <c r="F20" s="16" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="48"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="55" t="s">
+      <c r="A21" s="88"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="93" t="s">
         <v>157</v>
       </c>
-      <c r="D21" s="56"/>
-      <c r="E21" s="40" t="s">
+      <c r="D21" s="94"/>
+      <c r="E21" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="21" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="70" t="s">
         <v>218</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="70" t="s">
         <v>160</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="73" t="s">
         <v>161</v>
       </c>
-      <c r="D22" s="22"/>
+      <c r="D22" s="75"/>
       <c r="E22" s="8" t="s">
         <v>127</v>
       </c>
@@ -3935,10 +3941,10 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="24"/>
+      <c r="A23" s="72"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="96"/>
       <c r="E23" s="6" t="s">
         <v>102</v>
       </c>
@@ -3947,10 +3953,10 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="24"/>
+      <c r="A24" s="72"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="96"/>
       <c r="E24" s="6" t="s">
         <v>25</v>
       </c>
@@ -3959,10 +3965,10 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="24"/>
+      <c r="A25" s="72"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="96"/>
       <c r="E25" s="6" t="s">
         <v>133</v>
       </c>
@@ -3971,10 +3977,10 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="24"/>
+      <c r="A26" s="72"/>
+      <c r="B26" s="72"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="96"/>
       <c r="E26" s="6" t="s">
         <v>82</v>
       </c>
@@ -3983,32 +3989,32 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="24"/>
+      <c r="A27" s="72"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="96"/>
       <c r="E27" s="10"/>
       <c r="F27" s="7" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="26"/>
+      <c r="A28" s="72"/>
+      <c r="B28" s="72"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="78"/>
       <c r="E28" s="14"/>
       <c r="F28" s="7" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="21" t="s">
+      <c r="A29" s="72"/>
+      <c r="B29" s="72"/>
+      <c r="C29" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="D29" s="22"/>
+      <c r="D29" s="75"/>
       <c r="E29" s="13" t="s">
         <v>170</v>
       </c>
@@ -4017,10 +4023,10 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="24"/>
+      <c r="A30" s="72"/>
+      <c r="B30" s="72"/>
+      <c r="C30" s="95"/>
+      <c r="D30" s="96"/>
       <c r="E30" s="6" t="s">
         <v>25</v>
       </c>
@@ -4029,10 +4035,10 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="26"/>
+      <c r="A31" s="72"/>
+      <c r="B31" s="72"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="78"/>
       <c r="E31" s="6" t="s">
         <v>173</v>
       </c>
@@ -4041,12 +4047,12 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="21" t="s">
+      <c r="A32" s="72"/>
+      <c r="B32" s="72"/>
+      <c r="C32" s="73" t="s">
         <v>175</v>
       </c>
-      <c r="D32" s="22"/>
+      <c r="D32" s="75"/>
       <c r="E32" s="8" t="s">
         <v>176</v>
       </c>
@@ -4055,10 +4061,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="24"/>
+      <c r="A33" s="72"/>
+      <c r="B33" s="72"/>
+      <c r="C33" s="95"/>
+      <c r="D33" s="96"/>
       <c r="E33" s="6" t="s">
         <v>127</v>
       </c>
@@ -4067,10 +4073,10 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="24"/>
+      <c r="A34" s="72"/>
+      <c r="B34" s="72"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="96"/>
       <c r="E34" s="6" t="s">
         <v>102</v>
       </c>
@@ -4079,10 +4085,10 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="24"/>
+      <c r="A35" s="72"/>
+      <c r="B35" s="72"/>
+      <c r="C35" s="95"/>
+      <c r="D35" s="96"/>
       <c r="E35" s="6" t="s">
         <v>116</v>
       </c>
@@ -4091,10 +4097,10 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="24"/>
+      <c r="A36" s="72"/>
+      <c r="B36" s="72"/>
+      <c r="C36" s="95"/>
+      <c r="D36" s="96"/>
       <c r="E36" s="6" t="s">
         <v>102</v>
       </c>
@@ -4103,10 +4109,10 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="26"/>
+      <c r="A37" s="72"/>
+      <c r="B37" s="72"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="78"/>
       <c r="E37" s="6" t="s">
         <v>25</v>
       </c>
@@ -4115,12 +4121,12 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="21" t="s">
+      <c r="A38" s="72"/>
+      <c r="B38" s="72"/>
+      <c r="C38" s="73" t="s">
         <v>183</v>
       </c>
-      <c r="D38" s="22"/>
+      <c r="D38" s="75"/>
       <c r="E38" s="6" t="s">
         <v>184</v>
       </c>
@@ -4129,10 +4135,10 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="26"/>
+      <c r="A39" s="72"/>
+      <c r="B39" s="71"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="78"/>
       <c r="E39" s="6" t="s">
         <v>22</v>
       </c>
@@ -4141,12 +4147,12 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
-      <c r="B40" s="15" t="s">
+      <c r="A40" s="72"/>
+      <c r="B40" s="70" t="s">
         <v>186</v>
       </c>
-      <c r="C40" s="29"/>
-      <c r="D40" s="30"/>
+      <c r="C40" s="97"/>
+      <c r="D40" s="98"/>
       <c r="E40" s="8" t="s">
         <v>187</v>
       </c>
@@ -4155,10 +4161,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="16"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="32"/>
+      <c r="A41" s="72"/>
+      <c r="B41" s="72"/>
+      <c r="C41" s="99"/>
+      <c r="D41" s="100"/>
       <c r="E41" s="6" t="s">
         <v>187</v>
       </c>
@@ -4167,10 +4173,10 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="32"/>
+      <c r="A42" s="72"/>
+      <c r="B42" s="72"/>
+      <c r="C42" s="99"/>
+      <c r="D42" s="100"/>
       <c r="E42" s="6" t="s">
         <v>133</v>
       </c>
@@ -4179,10 +4185,10 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="34"/>
+      <c r="A43" s="72"/>
+      <c r="B43" s="72"/>
+      <c r="C43" s="101"/>
+      <c r="D43" s="102"/>
       <c r="E43" s="6" t="s">
         <v>191</v>
       </c>
@@ -4191,10 +4197,10 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="15" t="s">
+      <c r="A44" s="72"/>
+      <c r="B44" s="72"/>
+      <c r="C44" s="103"/>
+      <c r="D44" s="70" t="s">
         <v>193</v>
       </c>
       <c r="E44" s="8" t="s">
@@ -4205,10 +4211,10 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="17"/>
+      <c r="A45" s="72"/>
+      <c r="B45" s="71"/>
+      <c r="C45" s="104"/>
+      <c r="D45" s="71"/>
       <c r="E45" s="6" t="s">
         <v>102</v>
       </c>
@@ -4217,14 +4223,14 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
-      <c r="B46" s="15" t="s">
+      <c r="A46" s="72"/>
+      <c r="B46" s="70" t="s">
         <v>196</v>
       </c>
-      <c r="C46" s="21" t="s">
+      <c r="C46" s="73" t="s">
         <v>197</v>
       </c>
-      <c r="D46" s="22"/>
+      <c r="D46" s="75"/>
       <c r="E46" s="8" t="s">
         <v>60</v>
       </c>
@@ -4233,10 +4239,10 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="24"/>
+      <c r="A47" s="72"/>
+      <c r="B47" s="72"/>
+      <c r="C47" s="95"/>
+      <c r="D47" s="96"/>
       <c r="E47" s="6" t="s">
         <v>25</v>
       </c>
@@ -4245,10 +4251,10 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="16"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="24"/>
+      <c r="A48" s="72"/>
+      <c r="B48" s="72"/>
+      <c r="C48" s="95"/>
+      <c r="D48" s="96"/>
       <c r="E48" s="6" t="s">
         <v>25</v>
       </c>
@@ -4257,10 +4263,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
-      <c r="B49" s="16"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="26"/>
+      <c r="A49" s="72"/>
+      <c r="B49" s="72"/>
+      <c r="C49" s="76"/>
+      <c r="D49" s="78"/>
       <c r="E49" s="6" t="s">
         <v>133</v>
       </c>
@@ -4269,12 +4275,12 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="16"/>
-      <c r="B50" s="16"/>
-      <c r="C50" s="21" t="s">
+      <c r="A50" s="72"/>
+      <c r="B50" s="72"/>
+      <c r="C50" s="73" t="s">
         <v>202</v>
       </c>
-      <c r="D50" s="22"/>
+      <c r="D50" s="75"/>
       <c r="E50" s="8" t="s">
         <v>25</v>
       </c>
@@ -4283,11 +4289,11 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="16"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="15" t="s">
+      <c r="A51" s="72"/>
+      <c r="B51" s="72"/>
+      <c r="C51" s="95"/>
+      <c r="D51" s="96"/>
+      <c r="E51" s="70" t="s">
         <v>133</v>
       </c>
       <c r="F51" s="7" t="s">
@@ -4295,21 +4301,21 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="16"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="17"/>
+      <c r="A52" s="72"/>
+      <c r="B52" s="72"/>
+      <c r="C52" s="95"/>
+      <c r="D52" s="96"/>
+      <c r="E52" s="71"/>
       <c r="F52" s="7" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="16"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="15" t="s">
+      <c r="A53" s="72"/>
+      <c r="B53" s="72"/>
+      <c r="C53" s="95"/>
+      <c r="D53" s="96"/>
+      <c r="E53" s="70" t="s">
         <v>22</v>
       </c>
       <c r="F53" s="7" t="s">
@@ -4317,40 +4323,40 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="16"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="16"/>
+      <c r="A54" s="72"/>
+      <c r="B54" s="72"/>
+      <c r="C54" s="95"/>
+      <c r="D54" s="96"/>
+      <c r="E54" s="72"/>
       <c r="F54" s="7" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="16"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="23"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="16"/>
+      <c r="A55" s="72"/>
+      <c r="B55" s="72"/>
+      <c r="C55" s="95"/>
+      <c r="D55" s="96"/>
+      <c r="E55" s="72"/>
       <c r="F55" s="7" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="16"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="24"/>
-      <c r="E56" s="17"/>
+      <c r="A56" s="72"/>
+      <c r="B56" s="72"/>
+      <c r="C56" s="95"/>
+      <c r="D56" s="96"/>
+      <c r="E56" s="71"/>
       <c r="F56" s="7" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="25"/>
-      <c r="D57" s="26"/>
+      <c r="A57" s="72"/>
+      <c r="B57" s="71"/>
+      <c r="C57" s="76"/>
+      <c r="D57" s="78"/>
       <c r="E57" s="6" t="s">
         <v>191</v>
       </c>
@@ -4359,12 +4365,12 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="16"/>
-      <c r="B58" s="21" t="s">
+      <c r="A58" s="72"/>
+      <c r="B58" s="73" t="s">
         <v>211</v>
       </c>
-      <c r="C58" s="27"/>
-      <c r="D58" s="22"/>
+      <c r="C58" s="74"/>
+      <c r="D58" s="75"/>
       <c r="E58" s="6" t="s">
         <v>212</v>
       </c>
@@ -4373,10 +4379,10 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="16"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="28"/>
-      <c r="D59" s="26"/>
+      <c r="A59" s="72"/>
+      <c r="B59" s="76"/>
+      <c r="C59" s="77"/>
+      <c r="D59" s="78"/>
       <c r="E59" s="6" t="s">
         <v>212</v>
       </c>
@@ -4385,12 +4391,12 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="17"/>
-      <c r="B60" s="18" t="s">
+      <c r="A60" s="71"/>
+      <c r="B60" s="79" t="s">
         <v>215</v>
       </c>
-      <c r="C60" s="19"/>
-      <c r="D60" s="20"/>
+      <c r="C60" s="80"/>
+      <c r="D60" s="81"/>
       <c r="E60" s="11" t="s">
         <v>44</v>
       </c>
@@ -4400,6 +4406,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A1:A14"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:B14"/>
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C40:D43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="B46:B57"/>
+    <mergeCell ref="C46:D49"/>
+    <mergeCell ref="C50:D57"/>
+    <mergeCell ref="D44:D45"/>
     <mergeCell ref="E51:E52"/>
     <mergeCell ref="E53:E56"/>
     <mergeCell ref="B58:D59"/>
@@ -4416,20 +4436,6 @@
     <mergeCell ref="C32:D37"/>
     <mergeCell ref="C38:D39"/>
     <mergeCell ref="B40:B45"/>
-    <mergeCell ref="C40:D43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="B46:B57"/>
-    <mergeCell ref="C46:D49"/>
-    <mergeCell ref="C50:D57"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="A1:A14"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:B14"/>
-    <mergeCell ref="C2:C11"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>